<commit_message>
Added Aruba-CX config from Aaron
</commit_message>
<xml_diff>
--- a/CUSTOMER - Wired 802.1X Configurations.xlsx
+++ b/CUSTOMER - Wired 802.1X Configurations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcourtney/Documents/Adoptiv/Projects/Adaptive/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcourtney/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B967631-2D1A-FB40-8F0D-DD3267182B5B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3943233F-F430-9A46-B3E2-674A5646A843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1260" windowWidth="25600" windowHeight="13860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="31760" windowHeight="19160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StartHere" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,23 @@
     <sheet name="Advanced Cisco Switch Configs" sheetId="15" r:id="rId3"/>
     <sheet name="Juniper EX Config" sheetId="2" r:id="rId4"/>
     <sheet name="HPE Provision Config" sheetId="17" r:id="rId5"/>
-    <sheet name="Aruba S-Series Config" sheetId="16" r:id="rId6"/>
-    <sheet name="Extreme EXOS 15- Config" sheetId="19" r:id="rId7"/>
-    <sheet name="Extreme EXOS 16+ Config" sheetId="18" r:id="rId8"/>
+    <sheet name="Aruba CX Config" sheetId="20" r:id="rId6"/>
+    <sheet name="Aruba S-Series Config" sheetId="16" r:id="rId7"/>
+    <sheet name="Extreme EXOS 15- Config" sheetId="19" r:id="rId8"/>
+    <sheet name="Extreme EXOS 16+ Config" sheetId="18" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -35,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="324">
   <si>
     <t>&lt;-- Fill in this field</t>
   </si>
@@ -391,9 +400,6 @@
     <t>TACACS+ / RADIUS Source Interface VLAN</t>
   </si>
   <si>
-    <t>Adaptive Communications</t>
-  </si>
-  <si>
     <t>Designed by:</t>
   </si>
   <si>
@@ -463,9 +469,6 @@
     <t>aaa port-access authenticator active</t>
   </si>
   <si>
-    <t>aaa accounting update periodic 2</t>
-  </si>
-  <si>
     <t>aaa authentication port-access eap-radius server-group "CP-RAD-Grp"</t>
   </si>
   <si>
@@ -772,13 +775,247 @@
     <t>Guest VLAN Configuration</t>
   </si>
   <si>
-    <t>Mike Courtney</t>
-  </si>
-  <si>
-    <t>Updated: 01/02/2017</t>
-  </si>
-  <si>
     <t>aaa authorization auth-proxy default group radius</t>
+  </si>
+  <si>
+    <t>Dynamic Segmentation Per User Tunnel</t>
+  </si>
+  <si>
+    <t>aaa authorization user-role name &lt;name of role&gt; vlan-id &lt;vlan ID&gt;</t>
+  </si>
+  <si>
+    <t>aaa authorization user-role name &lt;name of role on switch&gt; tunneled-node-server-redirect secondary-role &lt;name of role on controller&gt;</t>
+  </si>
+  <si>
+    <t>tunneled-node-server controllier-ip &lt;controller IP&gt;</t>
+  </si>
+  <si>
+    <t>ip client-tracker trusted</t>
+  </si>
+  <si>
+    <t>aaa authentication captive-portal enable</t>
+  </si>
+  <si>
+    <t>aaa authorization user-role enable download</t>
+  </si>
+  <si>
+    <t>aaa accounting update periodic 5</t>
+  </si>
+  <si>
+    <t>Commands Used For Per User Tunnel</t>
+  </si>
+  <si>
+    <t>Commands Used For Per Port Tunnel</t>
+  </si>
+  <si>
+    <t>class ipv4 &lt;name of acl&gt;</t>
+  </si>
+  <si>
+    <t>match &lt;protocol&gt; &lt;src&gt; &lt;destination&gt; eq &lt;port #&gt;</t>
+  </si>
+  <si>
+    <t>policy user &lt;name of policy&gt;</t>
+  </si>
+  <si>
+    <t>class ipv4 &lt;name of acl&gt; action &lt;permit/deny&gt;</t>
+  </si>
+  <si>
+    <t>aaa authorization user-role name &lt;name of user role&gt;</t>
+  </si>
+  <si>
+    <t>policy &lt;name of policy&gt;</t>
+  </si>
+  <si>
+    <t>reauth-period &lt;time in seconds&gt;</t>
+  </si>
+  <si>
+    <t>vlan-name (or) vlan-id &lt;vlan name or id&gt;</t>
+  </si>
+  <si>
+    <t>captive-portal-profile use-radius-vsa</t>
+  </si>
+  <si>
+    <t>&lt;--- If you are using a captive portal</t>
+  </si>
+  <si>
+    <t>Download Root Cert From ClearPass</t>
+  </si>
+  <si>
+    <t>crypto ca-download usage clearpass retry 3</t>
+  </si>
+  <si>
+    <t>tunneled-node-server mode role-based reserved-vlan &lt;vlan-id&gt;</t>
+  </si>
+  <si>
+    <t>Copy and paste the following commands into the HPE Aruba-OS-CX CLI (version 16.4.+)</t>
+  </si>
+  <si>
+    <t>radius dyn-authorization enable</t>
+  </si>
+  <si>
+    <t>aaa group server radius CP-RAD-Grp</t>
+  </si>
+  <si>
+    <t>aaa group server tacacs CP-TAC-Grp</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access dot1x authenticator enable</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access dot1x authenticator auth-method eap-radius</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access dot1x authenticator radius server-group CP-RAD-Grp</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access mac-auth enable</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access mac-auth auth-method chap</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access mac-auth radius server-group CP-RAD-Grp</t>
+  </si>
+  <si>
+    <t>aaa authentication login console group radius local</t>
+  </si>
+  <si>
+    <t>aaa authentication login ssh group radius local</t>
+  </si>
+  <si>
+    <t>aaa authentication login https-server group radius local</t>
+  </si>
+  <si>
+    <t>aaa accounting port-access start-stop interim 1 group radius</t>
+  </si>
+  <si>
+    <t>aaa accounting all-mgmt console start-stop group radius</t>
+  </si>
+  <si>
+    <t>aaa accounting all-mgmt https-server start-stop group radius</t>
+  </si>
+  <si>
+    <t>aaa accounting all-mgmt ssh start-stop group radius</t>
+  </si>
+  <si>
+    <t>aaa accounting all-mgmt default start-stop group radius</t>
+  </si>
+  <si>
+    <t>no routing</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access dot1x authenticator eapol-timeout 10</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access client-limit 10</t>
+  </si>
+  <si>
+    <t>aaa authentication port-access auth-precedence mac-auth dot1x</t>
+  </si>
+  <si>
+    <t>no shutdown</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>Updated: 02/10/2020</t>
+  </si>
+  <si>
+    <t>aaa authorization commands console group tacacs local</t>
+  </si>
+  <si>
+    <t>TACACS+ Command Authorization</t>
+  </si>
+  <si>
+    <t>Commands Used For Per User-Role Based Enforcement</t>
+  </si>
+  <si>
+    <t>port-access role &lt;role_name&gt;</t>
+  </si>
+  <si>
+    <t>auth-mode client-mode</t>
+  </si>
+  <si>
+    <t>vlan access &lt;vlan-id&gt;</t>
+  </si>
+  <si>
+    <t>show aaa authentication port-access interface all clients-status</t>
+  </si>
+  <si>
+    <t>show port-access role radius</t>
+  </si>
+  <si>
+    <t>show port-access role name &lt;role_name&gt;</t>
+  </si>
+  <si>
+    <t>ubt-client-vlan 1000</t>
+  </si>
+  <si>
+    <t>ubt zone user vrf default</t>
+  </si>
+  <si>
+    <t>primary-controller ip &lt;mobility_controller_ip&gt;</t>
+  </si>
+  <si>
+    <t>sac-heartbeat-interval 1</t>
+  </si>
+  <si>
+    <t>uac-keepalive-interval 60</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>gateway-zone zone user gateway-role &lt;role_name_on_controller&gt;</t>
+  </si>
+  <si>
+    <t>port-access role &lt;role_name_on_switch&gt;</t>
+  </si>
+  <si>
+    <t>show ubt brief</t>
+  </si>
+  <si>
+    <t>show ubt users all</t>
+  </si>
+  <si>
+    <t>show ubt state</t>
+  </si>
+  <si>
+    <t>Commands Used for User Based Tunneling</t>
+  </si>
+  <si>
+    <t>ip dns server-address &lt;dns_ipaddress&gt;</t>
+  </si>
+  <si>
+    <t>ntp server &lt;ntp_server&gt;</t>
+  </si>
+  <si>
+    <t>ntp enable</t>
+  </si>
+  <si>
+    <t>crypto pki ta-profile &lt;profile_name&gt;</t>
+  </si>
+  <si>
+    <t>ta-certificate &lt;copy_paste_the_root_certificate&gt;</t>
+  </si>
+  <si>
+    <t>Commands Needed For Downloadable User-Roles to Work</t>
+  </si>
+  <si>
+    <t>radius-server host &lt;dns_name_of_ClearPass_server&gt; key plaintext &lt;radius-key&gt; clearpass-username &lt;user-name&gt; clearpass-password plaintext &lt;password&gt;</t>
+  </si>
+  <si>
+    <t>NorthStar Networks</t>
+  </si>
+  <si>
+    <t>Mike Courtney - mike@northstarnetworks.com</t>
+  </si>
+  <si>
+    <t>Aruba Networks</t>
+  </si>
+  <si>
+    <t>Aaron X. Smith - aaron.x.smith@hpe.com</t>
   </si>
 </sst>
 </file>
@@ -910,8 +1147,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="195">
+  <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1157,7 +1396,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="195">
+  <cellStyles count="197">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1255,6 +1494,7 @@
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1352,6 +1592,7 @@
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1691,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:MC108"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="MC108" sqref="MC108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1710,7 +1951,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1721,7 +1962,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1732,7 +1973,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1768,7 +2009,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1779,7 +2020,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1845,7 +2086,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="8" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="B39" s="4"/>
     </row>
@@ -1882,24 +2123,28 @@
     </row>
     <row r="103" spans="341:341">
       <c r="MC103" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="341:341">
       <c r="MC104" s="1" t="s">
-        <v>245</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" spans="341:341">
       <c r="MC105" s="1" t="s">
-        <v>118</v>
+        <v>320</v>
       </c>
     </row>
     <row r="107" spans="341:341">
-      <c r="MC107" s="1"/>
+      <c r="MC107" s="1" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="108" spans="341:341">
-      <c r="MC108" s="1"/>
+      <c r="MC108" s="1" t="s">
+        <v>322</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
@@ -1919,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1931,10 +2176,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19">
@@ -1942,7 +2187,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19">
@@ -1953,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19">
@@ -1961,7 +2206,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1970,7 +2215,7 @@
         <v xml:space="preserve">tacacs-server host </v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1979,7 +2224,7 @@
         <v xml:space="preserve">tacacs-server host </v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1987,7 +2232,7 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1995,7 +2240,7 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2015,7 +2260,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2030,7 +2275,7 @@
         <v xml:space="preserve">radius-server host  auth-port 1812 acct-port 1813 key </v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2045,7 +2290,7 @@
         <v xml:space="preserve">radius-server attribute 4 </v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2058,7 +2303,7 @@
         <v>45</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2071,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2085,7 +2330,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2093,15 +2338,15 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2109,7 +2354,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2117,7 +2362,7 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2130,7 +2375,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2143,7 +2388,7 @@
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2195,7 +2440,7 @@
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:1">
@@ -2693,10 +2938,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19">
@@ -2704,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2713,7 +2958,7 @@
         <v>set system radius-server  port 1812</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2722,7 +2967,7 @@
         <v>set system radius-server  accounting-port 1813</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2731,7 +2976,7 @@
         <v xml:space="preserve">set system radius-server  secret </v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2740,7 +2985,7 @@
         <v xml:space="preserve">set system radius-server  source-address </v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2749,7 +2994,7 @@
         <v>set system radius-server  port 1812</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2758,7 +3003,7 @@
         <v>set system radius-server  accounting-port 1813</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2786,7 +3031,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2801,7 +3046,7 @@
         <v xml:space="preserve">set system accounting destination radius server  secret </v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2816,7 +3061,7 @@
         <v>set system accounting destination radius server  accounting-port 1813</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2831,7 +3076,7 @@
         <v xml:space="preserve">set system accounting destination radius server  source-address </v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17">
@@ -2847,7 +3092,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2986,42 +3231,42 @@
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:1">
@@ -3029,7 +3274,7 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:1">
@@ -3149,10 +3394,829 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="129.83203125" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19">
+      <c r="A1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19">
+      <c r="A3" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A4," key ",StartHere!A10)</f>
+        <v xml:space="preserve">radius-server host  key </v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A4," dyn-authorization")</f>
+        <v>radius-server host  dyn-authorization</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A4," time-window 0")</f>
+        <v>radius-server host  time-window 0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A7," key ",StartHere!A10)</f>
+        <v xml:space="preserve">radius-server host  key </v>
+      </c>
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A7," dyn-authorization")</f>
+        <v>radius-server host  dyn-authorization</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A7," time-window 0")</f>
+        <v>radius-server host  time-window 0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="str">
+        <f>CONCATENATE("tacacs-server host ",StartHere!A4," key ",StartHere!A10)</f>
+        <v xml:space="preserve">tacacs-server host  key </v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="str">
+        <f>CONCATENATE("tacacs-server host ",StartHere!A7," key ",StartHere!A10)</f>
+        <v xml:space="preserve">tacacs-server host  key </v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="str">
+        <f>CONCATENATE("aaa server-group radius ""CP-RAD-Grp"" host ",StartHere!A4)</f>
+        <v xml:space="preserve">aaa server-group radius "CP-RAD-Grp" host </v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="str">
+        <f>CONCATENATE("aaa server-group radius ""CP-RAD-Grp"" host ",StartHere!A7)</f>
+        <v xml:space="preserve">aaa server-group radius "CP-RAD-Grp" host </v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="str">
+        <f>CONCATENATE("ip source-interface radius vlan ",StartHere!A16)</f>
+        <v xml:space="preserve">ip source-interface radius vlan </v>
+      </c>
+      <c r="B19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="str">
+        <f>CONCATENATE("ip source-interface tacacs vlan ",StartHere!A16)</f>
+        <v xml:space="preserve">ip source-interface tacacs vlan </v>
+      </c>
+      <c r="B20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="str">
+        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22)</f>
+        <v>aaa port-access authenticator -</v>
+      </c>
+      <c r="B24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="str">
+        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " supplicant-timeout 10")</f>
+        <v>aaa port-access authenticator - supplicant-timeout 10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="str">
+        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " tx-period 10")</f>
+        <v>aaa port-access authenticator - tx-period 10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="str">
+        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " logoff-period 862400")</f>
+        <v>aaa port-access authenticator - logoff-period 862400</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="str">
+        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " client-limit 10")</f>
+        <v>aaa port-access authenticator - client-limit 10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="str">
+        <f>CONCATENATE("aaa port-access mac-based ",StartHere!A19,"-",StartHere!A22)</f>
+        <v>aaa port-access mac-based -</v>
+      </c>
+      <c r="B29" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>227</v>
+      </c>
+      <c r="B42" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>231</v>
+      </c>
+      <c r="B44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>233</v>
+      </c>
+      <c r="B47" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>234</v>
+      </c>
+      <c r="B48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>236</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>249</v>
+      </c>
+      <c r="B51" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A4," clearpass")</f>
+        <v>radius-server host  clearpass</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="B52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="7"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="7"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="7"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="7"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="7"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="7"/>
+    </row>
+    <row r="83" spans="1:1" ht="19">
+      <c r="A83" s="12"/>
+    </row>
+    <row r="84" spans="1:1" ht="19">
+      <c r="A84" s="12"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:1" ht="19">
+      <c r="A87" s="12"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="13"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="91" spans="1:1" ht="19">
+      <c r="A91" s="14"/>
+    </row>
+    <row r="93" spans="1:1" ht="19">
+      <c r="A93" s="5"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" ht="19">
+      <c r="A100" s="5"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="4"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="4"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="4"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="4"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="4"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51539DD6-84D9-4742-ACC1-BA0B3E1A9368}">
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="128.6640625" customWidth="1"/>
+    <col min="2" max="2" width="134" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19">
+      <c r="A1" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19">
+      <c r="A3" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="str">
+        <f>CONCATENATE("radius dyn-authorization client ",StartHere!A4," secret-key plaintext ",StartHere!A10," time-window 1")</f>
+        <v>radius dyn-authorization client  secret-key plaintext  time-window 1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="str">
+        <f>CONCATENATE("radius dyn-authorization client ",StartHere!A7," secret-key plaintext ",StartHere!A10," time-window 1")</f>
+        <v>radius dyn-authorization client  secret-key plaintext  time-window 1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A4," key plaintext ",StartHere!A10,"")</f>
+        <v xml:space="preserve">radius-server host  key plaintext </v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="str">
+        <f>CONCATENATE("radius-server host ",StartHere!A7," key plaintext ",StartHere!A10,"")</f>
+        <v xml:space="preserve">radius-server host  key plaintext </v>
+      </c>
+      <c r="B9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="str">
+        <f>CONCATENATE("tacacs-server host ",StartHere!A4," key plaintext ",StartHere!A10,"")</f>
+        <v xml:space="preserve">tacacs-server host  key plaintext </v>
+      </c>
+      <c r="B11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="str">
+        <f>CONCATENATE("tacacs-server host ",StartHere!A7," key plaintext ",StartHere!A10,"")</f>
+        <v xml:space="preserve">tacacs-server host  key plaintext </v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="str">
+        <f>CONCATENATE("server ",StartHere!A4,"")</f>
+        <v xml:space="preserve">server </v>
+      </c>
+      <c r="B15" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="str">
+        <f>CONCATENATE("server ",StartHere!A7,"")</f>
+        <v xml:space="preserve">server </v>
+      </c>
+      <c r="B16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="str">
+        <f>CONCATENATE("server ",StartHere!A4,"")</f>
+        <v xml:space="preserve">server </v>
+      </c>
+      <c r="B18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="str">
+        <f>CONCATENATE("server ",StartHere!A7,"")</f>
+        <v xml:space="preserve">server </v>
+      </c>
+      <c r="B19" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="str">
+        <f>CONCATENATE("ip source-interface radius ",StartHere!A13,"")</f>
+        <v xml:space="preserve">ip source-interface radius </v>
+      </c>
+      <c r="B22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="str">
+        <f>CONCATENATE("ip source-interface tacacs ",StartHere!A13,"")</f>
+        <v xml:space="preserve">ip source-interface tacacs </v>
+      </c>
+      <c r="B23" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>276</v>
+      </c>
+      <c r="B30" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>278</v>
+      </c>
+      <c r="B33" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>279</v>
+      </c>
+      <c r="B34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19">
+      <c r="A37" t="s">
+        <v>281</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>283</v>
+      </c>
+      <c r="B39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B40" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="B41" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="str">
+        <f>CONCATENATE("interface ",StartHere!A19,"-",StartHere!A22,"")</f>
+        <v>interface -</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B43" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>285</v>
+      </c>
+      <c r="B44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>271</v>
+      </c>
+      <c r="B45" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B136"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3163,86 +4227,80 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>194</v>
-      </c>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2" ht="19">
-      <c r="A3" s="6" t="s">
-        <v>149</v>
+      <c r="A3" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="str">
-        <f>CONCATENATE("radius-server host ",StartHere!A4," key ",StartHere!A10)</f>
-        <v xml:space="preserve">radius-server host  key </v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19">
+      <c r="A5" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="str">
-        <f>CONCATENATE("radius-server host ",StartHere!A4," dyn-authorization")</f>
-        <v>radius-server host  dyn-authorization</v>
-      </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="str">
-        <f>CONCATENATE("radius-server host ",StartHere!A4," time-window 0")</f>
-        <v>radius-server host  time-window 0</v>
+      <c r="A7" t="s">
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="str">
-        <f>CONCATENATE("radius-server host ",StartHere!A7," key ",StartHere!A10)</f>
-        <v xml:space="preserve">radius-server host  key </v>
+        <f>CONCATENATE("   host ",StartHere!A4,"")</f>
+        <v xml:space="preserve">   host </v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="str">
-        <f>CONCATENATE("radius-server host ",StartHere!A7," dyn-authorization")</f>
-        <v>radius-server host  dyn-authorization</v>
+        <f>CONCATENATE("   key ",StartHere!A10)</f>
+        <v xml:space="preserve">   key </v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="str">
-        <f>CONCATENATE("radius-server host ",StartHere!A7," time-window 0")</f>
-        <v>radius-server host  time-window 0</v>
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="str">
-        <f>CONCATENATE("tacacs-server host ",StartHere!A4," key ",StartHere!A10)</f>
-        <v xml:space="preserve">tacacs-server host  key </v>
+        <f>CONCATENATE("   host ",StartHere!A7,"")</f>
+        <v xml:space="preserve">   host </v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="str">
-        <f>CONCATENATE("tacacs-server host ",StartHere!A7," key ",StartHere!A10)</f>
-        <v xml:space="preserve">tacacs-server host  key </v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>244</v>
+        <f>CONCATENATE("   key ",StartHere!A10)</f>
+        <v xml:space="preserve">   key </v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3252,308 +4310,442 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="str">
-        <f>CONCATENATE("aaa server-group radius ""CP-RAD-Grp"" host ",StartHere!A4)</f>
-        <v xml:space="preserve">aaa server-group radius "CP-RAD-Grp" host </v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>217</v>
+        <f>CONCATENATE("aaa rfc-3576-server ",StartHere!A4)</f>
+        <v xml:space="preserve">aaa rfc-3576-server </v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="str">
-        <f>CONCATENATE("aaa server-group radius ""CP-RAD-Grp"" host ",StartHere!A7)</f>
-        <v xml:space="preserve">aaa server-group radius "CP-RAD-Grp" host </v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <f>CONCATENATE("   key ",StartHere!A10)</f>
+        <v xml:space="preserve">   key </v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" t="str">
-        <f>CONCATENATE("ip source-interface radius vlan ",StartHere!A16)</f>
-        <v xml:space="preserve">ip source-interface radius vlan </v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <f>CONCATENATE("aaa rfc-3576-server ",StartHere!A7)</f>
+        <v xml:space="preserve">aaa rfc-3576-server </v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" t="str">
-        <f>CONCATENATE("ip source-interface tacacs vlan ",StartHere!A16)</f>
-        <v xml:space="preserve">ip source-interface tacacs vlan </v>
-      </c>
-      <c r="B19" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <f>CONCATENATE("   key ",StartHere!A10)</f>
+        <v xml:space="preserve">   key </v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="str">
-        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22)</f>
-        <v>aaa port-access authenticator -</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="str">
-        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " quiet-period 30")</f>
-        <v>aaa port-access authenticator - quiet-period 30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="str">
-        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " logoff-period 862400")</f>
-        <v>aaa port-access authenticator - logoff-period 862400</v>
-      </c>
-      <c r="B25" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <f>CONCATENATE("ip radius source-interface vlan ",StartHere!A16)</f>
+        <v xml:space="preserve">ip radius source-interface vlan </v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26" t="str">
-        <f>CONCATENATE("aaa port-access authenticator ",StartHere!A19,"-",StartHere!A22, " client-limit 2")</f>
-        <v>aaa port-access authenticator - client-limit 2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="str">
-        <f>CONCATENATE("aaa port-access mac-based ",StartHere!A19,"-",StartHere!A22)</f>
-        <v>aaa port-access mac-based -</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <f>CONCATENATE("ip radius nas-ip ",StartHere!A13)</f>
+        <v xml:space="preserve">ip radius nas-ip </v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="str">
+        <f>CONCATENATE("   host ",StartHere!A4,"")</f>
+        <v xml:space="preserve">   host </v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="str">
+        <f>CONCATENATE("   key ",StartHere!A10)</f>
+        <v xml:space="preserve">   key </v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>147</v>
+      <c r="A33" t="str">
+        <f>CONCATENATE("   host ",StartHere!A7,"")</f>
+        <v xml:space="preserve">   host </v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>148</v>
+      <c r="A34" t="str">
+        <f>CONCATENATE("   key ",StartHere!A10)</f>
+        <v xml:space="preserve">   key </v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>229</v>
+      <c r="A40" t="str">
+        <f>CONCATENATE("ip tacacs source-interface vlan ",StartHere!A16)</f>
+        <v xml:space="preserve">ip tacacs source-interface vlan </v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>230</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>233</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>240</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>234</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>237</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>238</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="7"/>
+      <c r="A55" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="7"/>
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="7"/>
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="7"/>
+      <c r="A58" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="7"/>
+      <c r="A59" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="7"/>
+      <c r="A60" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="7"/>
+      <c r="A61" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="7"/>
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="7"/>
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="7"/>
+      <c r="A64" t="str">
+        <f>CONCATENATE("   rfc-3576-server ",StartHere!A4)</f>
+        <v xml:space="preserve">   rfc-3576-server </v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="str">
+        <f>CONCATENATE("   rfc-3576-server ",StartHere!A7)</f>
+        <v xml:space="preserve">   rfc-3576-server </v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="7"/>
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="7"/>
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="7"/>
+      <c r="A69" t="str">
+        <f>CONCATENATE("   apply-to ",StartHere!A19,"-",StartHere!A22)</f>
+        <v xml:space="preserve">   apply-to -</v>
+      </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="7"/>
-    </row>
-    <row r="81" spans="1:1" ht="19">
-      <c r="A81" s="12"/>
-    </row>
-    <row r="82" spans="1:1" ht="19">
-      <c r="A82" s="12"/>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="4"/>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="4"/>
-    </row>
-    <row r="85" spans="1:1" ht="19">
-      <c r="A85" s="12"/>
+      <c r="A70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="13"/>
+      <c r="A86" s="7"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="4"/>
-    </row>
-    <row r="89" spans="1:1" ht="19">
-      <c r="A89" s="14"/>
-    </row>
-    <row r="91" spans="1:1" ht="19">
-      <c r="A91" s="5"/>
+      <c r="A87" s="7"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="7"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="7"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="7"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="7"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="1"/>
+      <c r="A92" s="7"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="3"/>
+      <c r="A93" s="7"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="3"/>
+      <c r="A94" s="7"/>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="3"/>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="3"/>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="3"/>
-    </row>
-    <row r="98" spans="1:1" ht="19">
-      <c r="A98" s="5"/>
+      <c r="A95" s="7"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="7"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="7"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="4"/>
+      <c r="A100" s="7"/>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="4"/>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="4"/>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="4"/>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="4"/>
+      <c r="A101" s="7"/>
+    </row>
+    <row r="112" spans="1:1" ht="19">
+      <c r="A112" s="12"/>
+    </row>
+    <row r="113" spans="1:1" ht="19">
+      <c r="A113" s="12"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="4"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116" spans="1:1" ht="19">
+      <c r="A116" s="12"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="13"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="4"/>
+    </row>
+    <row r="120" spans="1:1" ht="19">
+      <c r="A120" s="14"/>
+    </row>
+    <row r="122" spans="1:1" ht="19">
+      <c r="A122" s="5"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="3"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="3"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="3"/>
+    </row>
+    <row r="129" spans="1:1" ht="19">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="4"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="4"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="4"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -3562,550 +4754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B136"/>
-  <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:A78"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="129.83203125" customWidth="1"/>
-    <col min="2" max="2" width="65.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="19">
-      <c r="A1" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="19">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:2" ht="19">
-      <c r="A3" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19">
-      <c r="A5" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="str">
-        <f>CONCATENATE("   host ",StartHere!A4,"")</f>
-        <v xml:space="preserve">   host </v>
-      </c>
-      <c r="B8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="str">
-        <f>CONCATENATE("   key ",StartHere!A10)</f>
-        <v xml:space="preserve">   key </v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="str">
-        <f>CONCATENATE("   host ",StartHere!A7,"")</f>
-        <v xml:space="preserve">   host </v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="str">
-        <f>CONCATENATE("   key ",StartHere!A10)</f>
-        <v xml:space="preserve">   key </v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="str">
-        <f>CONCATENATE("aaa rfc-3576-server ",StartHere!A4)</f>
-        <v xml:space="preserve">aaa rfc-3576-server </v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="str">
-        <f>CONCATENATE("   key ",StartHere!A10)</f>
-        <v xml:space="preserve">   key </v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="str">
-        <f>CONCATENATE("aaa rfc-3576-server ",StartHere!A7)</f>
-        <v xml:space="preserve">aaa rfc-3576-server </v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="str">
-        <f>CONCATENATE("   key ",StartHere!A10)</f>
-        <v xml:space="preserve">   key </v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="str">
-        <f>CONCATENATE("ip radius source-interface vlan ",StartHere!A16)</f>
-        <v xml:space="preserve">ip radius source-interface vlan </v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="str">
-        <f>CONCATENATE("ip radius nas-ip ",StartHere!A13)</f>
-        <v xml:space="preserve">ip radius nas-ip </v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="str">
-        <f>CONCATENATE("   host ",StartHere!A4,"")</f>
-        <v xml:space="preserve">   host </v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="str">
-        <f>CONCATENATE("   key ",StartHere!A10)</f>
-        <v xml:space="preserve">   key </v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="str">
-        <f>CONCATENATE("   host ",StartHere!A7,"")</f>
-        <v xml:space="preserve">   host </v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="str">
-        <f>CONCATENATE("   key ",StartHere!A10)</f>
-        <v xml:space="preserve">   key </v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="str">
-        <f>CONCATENATE("ip tacacs source-interface vlan ",StartHere!A16)</f>
-        <v xml:space="preserve">ip tacacs source-interface vlan </v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="str">
-        <f>CONCATENATE("   rfc-3576-server ",StartHere!A4)</f>
-        <v xml:space="preserve">   rfc-3576-server </v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="str">
-        <f>CONCATENATE("   rfc-3576-server ",StartHere!A7)</f>
-        <v xml:space="preserve">   rfc-3576-server </v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="str">
-        <f>CONCATENATE("   apply-to ",StartHere!A19,"-",StartHere!A22)</f>
-        <v xml:space="preserve">   apply-to -</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="7"/>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="7"/>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="7"/>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="7"/>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="7"/>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="7"/>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="7"/>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="7"/>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="7"/>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="7"/>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="7"/>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="7"/>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="7"/>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="7"/>
-    </row>
-    <row r="112" spans="1:1" ht="19">
-      <c r="A112" s="12"/>
-    </row>
-    <row r="113" spans="1:1" ht="19">
-      <c r="A113" s="12"/>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="4"/>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" s="4"/>
-    </row>
-    <row r="116" spans="1:1" ht="19">
-      <c r="A116" s="12"/>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" s="13"/>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" s="4"/>
-    </row>
-    <row r="120" spans="1:1" ht="19">
-      <c r="A120" s="14"/>
-    </row>
-    <row r="122" spans="1:1" ht="19">
-      <c r="A122" s="5"/>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" s="3"/>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" s="3"/>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" s="3"/>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" s="3"/>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" s="3"/>
-    </row>
-    <row r="129" spans="1:1" ht="19">
-      <c r="A129" s="5"/>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" s="4"/>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" s="4"/>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" s="4"/>
-    </row>
-    <row r="134" spans="1:1">
-      <c r="A134" s="4"/>
-    </row>
-    <row r="136" spans="1:1">
-      <c r="A136" s="4"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B123"/>
   <sheetViews>
@@ -4121,18 +4770,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19">
       <c r="A3" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19">
@@ -4144,7 +4793,7 @@
         <v>configure radius mgmt-access primary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4153,7 +4802,7 @@
         <v xml:space="preserve">configure radius mgmt-access primary shared-secret </v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4162,7 +4811,7 @@
         <v>configure radius mgmt-access secondary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4171,7 +4820,7 @@
         <v xml:space="preserve">configure radius mgmt-access secondary shared-secret </v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4180,7 +4829,7 @@
         <v>configure radius netlogin primary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4189,7 +4838,7 @@
         <v xml:space="preserve">configure radius netlogin primary shared-secret </v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4210,7 +4859,7 @@
         <v>configure radius-accounting mgmt-access primary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4225,7 +4874,7 @@
         <v>configure radius-accounting mgmt-access secondary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4246,7 +4895,7 @@
         <v xml:space="preserve">configure radius-accounting netlogin primary shared-secret </v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4261,12 +4910,12 @@
         <v xml:space="preserve">configure radius-accounting netlogin secondary shared-secret </v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4275,7 +4924,7 @@
         <v>configure tacacs primary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4290,7 +4939,7 @@
         <v xml:space="preserve">configure tacacs primary shared-secret </v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4325,37 +4974,37 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:1">
@@ -4390,27 +5039,27 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -4522,7 +5171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B120"/>
   <sheetViews>
@@ -4538,18 +5187,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19">
       <c r="A3" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19">
@@ -4561,7 +5210,7 @@
         <v>configure radius mgmt-access primary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4570,7 +5219,7 @@
         <v>configure radius mgmt-access secondary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4579,7 +5228,7 @@
         <v>configure radius netlogin primary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4588,7 +5237,7 @@
         <v>configure radius netlogin secondary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4597,7 +5246,7 @@
         <v>configure vm-tracking nms primary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4606,7 +5255,7 @@
         <v>configure vm-tracking nms secondary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4633,12 +5282,12 @@
         <v>configure radius-accounting netlogin secondary server  client-ip  shared-secret  vr VR-Default</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4647,7 +5296,7 @@
         <v>configure tacacs primary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4668,7 +5317,7 @@
         <v xml:space="preserve">configure tacacs secondary shared-secret </v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4683,7 +5332,7 @@
         <v>configure tacacs-accounting secondary server  client-ip  vr VR-Default</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4698,35 +5347,35 @@
         <v xml:space="preserve">configure tacacs-accounting secondary shared-secret </v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4737,17 +5386,17 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -4788,27 +5437,27 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:1">

</xml_diff>